<commit_message>
Reading from database included and there is analysis of 5 company ID's
</commit_message>
<xml_diff>
--- a/data/2/samplepnl.xlsx
+++ b/data/2/samplepnl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\28rac\Desktop\hybrid_chatbot\data\2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4A596A-BCAC-4024-BA64-FA412D0D0801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359B86D4-3E08-4821-8BC8-DA8424C5D56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="2850" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <r>
       <rPr>
@@ -139,28 +139,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Business Income</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Services</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>Total Income</t>
     </r>
   </si>
@@ -216,28 +194,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Office Rent</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Repairs &amp; maintenance</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>Utilities</t>
     </r>
   </si>
@@ -249,28 +205,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Internet &amp; TV services</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Phone service</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>Total Utilities</t>
     </r>
   </si>
@@ -304,61 +238,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Bank fees &amp; service charges</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Contributions to charities</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Office supplies</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Shipping &amp; postage</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Software &amp; apps</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>Total General business expenses</t>
     </r>
   </si>
@@ -381,28 +260,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Meals with clients</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Travel meals</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>Total Meals</t>
     </r>
   </si>
@@ -436,83 +293,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Continuing education</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Employee retirement plans (deleted)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Employer Taxes</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Health insurance &amp; accident plans</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Payroll Service fee</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Pension Expense</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Salaries &amp; wages</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>Total Personnel Expenses</t>
     </r>
   </si>
@@ -535,39 +315,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Accounting fees</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Dues &amp; subscriptions</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Legal Fees</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>Total Professional Services</t>
     </r>
   </si>
@@ -590,17 +337,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Business licenses</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>Total Taxes &amp; License</t>
     </r>
   </si>
@@ -612,50 +348,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Travel</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Airfare</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Hotels</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Taxis or shared rides</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>Total Travel</t>
     </r>
   </si>
@@ -678,50 +370,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Vehicle gas &amp; fuel</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Vehicle insurance</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Vehicle registration</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Vehicle wash &amp; road services</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="7.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>Total Vehicle expenses</t>
     </r>
   </si>
@@ -769,10 +417,103 @@
     </r>
   </si>
   <si>
-    <t>Advertising &amp; marketing</t>
-  </si>
-  <si>
-    <t>Category</t>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d </t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f </t>
+  </si>
+  <si>
+    <t xml:space="preserve">g </t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i </t>
+  </si>
+  <si>
+    <t xml:space="preserve">j </t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l </t>
+  </si>
+  <si>
+    <t xml:space="preserve">m </t>
+  </si>
+  <si>
+    <t xml:space="preserve">n </t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u </t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Travel</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>d1</t>
+  </si>
+  <si>
+    <t>e1</t>
+  </si>
+  <si>
+    <t>f1</t>
+  </si>
+  <si>
+    <t>g1</t>
   </si>
 </sst>
 </file>
@@ -906,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -967,9 +708,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
@@ -996,6 +734,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1304,7 +1048,7 @@
   <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1318,42 +1062,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
     </row>
     <row r="3" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
     </row>
     <row r="4" spans="1:7" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1385,8 +1127,8 @@
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>10</v>
+      <c r="A6" s="25" t="s">
+        <v>36</v>
       </c>
       <c r="B6" s="8">
         <v>18672.509999999998</v>
@@ -1408,8 +1150,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="14.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>11</v>
+      <c r="A7" s="25" t="s">
+        <v>37</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -1426,7 +1168,7 @@
     </row>
     <row r="8" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="11">
         <v>18672.509999999998</v>
@@ -1444,12 +1186,12 @@
         <v>11989.19</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="14">
         <v>18672.509999999998</v>
@@ -1467,12 +1209,12 @@
         <v>11989.19</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -1482,8 +1224,8 @@
       <c r="G10" s="17"/>
     </row>
     <row r="11" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
-        <v>68</v>
+      <c r="A11" s="25" t="s">
+        <v>38</v>
       </c>
       <c r="B11" s="18">
         <v>271.24</v>
@@ -1506,7 +1248,7 @@
     </row>
     <row r="12" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
@@ -1518,8 +1260,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
-        <v>17</v>
+      <c r="A13" s="29" t="s">
+        <v>39</v>
       </c>
       <c r="B13" s="18">
         <v>624</v>
@@ -1541,8 +1283,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
-        <v>18</v>
+      <c r="A14" s="29" t="s">
+        <v>40</v>
       </c>
       <c r="B14" s="8">
         <v>2075.84</v>
@@ -1565,7 +1307,7 @@
     </row>
     <row r="15" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="18">
@@ -1579,8 +1321,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
-        <v>20</v>
+      <c r="A16" s="30" t="s">
+        <v>41</v>
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
@@ -1594,45 +1336,45 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="14.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="21">
+      <c r="A17" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="20">
         <v>140.94999999999999</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="20">
         <v>140.96</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17" s="20">
         <v>140.96</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="20">
         <v>140.97</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="20">
         <v>145.78</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="20">
         <v>709.62</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="22">
+        <v>16</v>
+      </c>
+      <c r="B18" s="21">
         <v>140.94999999999999</v>
       </c>
-      <c r="C18" s="23">
+      <c r="C18" s="22">
         <v>438.51</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="22">
         <v>140.96</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="22">
         <v>140.97</v>
       </c>
-      <c r="F18" s="22">
+      <c r="F18" s="21">
         <v>771.83</v>
       </c>
       <c r="G18" s="11">
@@ -1641,7 +1383,7 @@
     </row>
     <row r="19" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B19" s="14">
         <v>2840.79</v>
@@ -1649,7 +1391,7 @@
       <c r="C19" s="15">
         <v>2374.96</v>
       </c>
-      <c r="D19" s="24">
+      <c r="D19" s="23">
         <v>795.73</v>
       </c>
       <c r="E19" s="15">
@@ -1664,7 +1406,7 @@
     </row>
     <row r="20" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -1676,8 +1418,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="19" t="s">
-        <v>25</v>
+      <c r="A21" s="29" t="s">
+        <v>43</v>
       </c>
       <c r="B21" s="18">
         <v>220.24</v>
@@ -1699,8 +1441,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="19" t="s">
-        <v>26</v>
+      <c r="A22" s="29" t="s">
+        <v>44</v>
       </c>
       <c r="B22" s="17"/>
       <c r="C22" s="18">
@@ -1714,8 +1456,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="19" t="s">
-        <v>27</v>
+      <c r="A23" s="29" t="s">
+        <v>45</v>
       </c>
       <c r="B23" s="18">
         <v>458.14</v>
@@ -1737,8 +1479,8 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="19" t="s">
-        <v>28</v>
+      <c r="A24" s="29" t="s">
+        <v>46</v>
       </c>
       <c r="B24" s="17"/>
       <c r="C24" s="18">
@@ -1754,22 +1496,22 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="14.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="21">
+      <c r="A25" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="20">
         <v>278.98</v>
       </c>
       <c r="C25" s="10">
         <v>1173.4000000000001</v>
       </c>
-      <c r="D25" s="21">
+      <c r="D25" s="20">
         <v>586.49</v>
       </c>
-      <c r="E25" s="21">
+      <c r="E25" s="20">
         <v>529.16999999999996</v>
       </c>
-      <c r="F25" s="21">
+      <c r="F25" s="20">
         <v>372.42</v>
       </c>
       <c r="G25" s="10">
@@ -1778,9 +1520,9 @@
     </row>
     <row r="26" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="25">
+        <v>19</v>
+      </c>
+      <c r="B26" s="24">
         <v>957.36</v>
       </c>
       <c r="C26" s="15">
@@ -1801,7 +1543,7 @@
     </row>
     <row r="27" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B27" s="18">
         <v>440.14</v>
@@ -1823,8 +1565,8 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="19" t="s">
-        <v>32</v>
+      <c r="A28" s="29" t="s">
+        <v>48</v>
       </c>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
@@ -1842,36 +1584,36 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="14.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="19" t="s">
-        <v>33</v>
+      <c r="A29" s="29" t="s">
+        <v>49</v>
       </c>
       <c r="B29" s="9"/>
-      <c r="C29" s="21">
+      <c r="C29" s="20">
         <v>5.6</v>
       </c>
       <c r="D29" s="9"/>
-      <c r="E29" s="21">
+      <c r="E29" s="20">
         <v>5.75</v>
       </c>
       <c r="F29" s="9"/>
-      <c r="G29" s="21">
+      <c r="G29" s="20">
         <v>11.35</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" s="25">
+        <v>21</v>
+      </c>
+      <c r="B30" s="24">
         <v>440.14</v>
       </c>
-      <c r="C30" s="24">
+      <c r="C30" s="23">
         <v>787.76</v>
       </c>
       <c r="D30" s="15">
         <v>1237.3499999999999</v>
       </c>
-      <c r="E30" s="24">
+      <c r="E30" s="23">
         <v>957.17</v>
       </c>
       <c r="F30" s="14">
@@ -1883,7 +1625,7 @@
     </row>
     <row r="31" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B31" s="18">
         <v>29.5</v>
@@ -1898,7 +1640,7 @@
     </row>
     <row r="32" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -1912,8 +1654,8 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="19" t="s">
-        <v>37</v>
+      <c r="A33" s="29" t="s">
+        <v>50</v>
       </c>
       <c r="B33" s="18">
         <v>5</v>
@@ -1935,8 +1677,8 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="19" t="s">
-        <v>38</v>
+      <c r="A34" s="29" t="s">
+        <v>51</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
@@ -1952,8 +1694,8 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="19" t="s">
-        <v>39</v>
+      <c r="A35" s="29" t="s">
+        <v>52</v>
       </c>
       <c r="B35" s="18">
         <v>475.5</v>
@@ -1969,8 +1711,8 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="19" t="s">
-        <v>40</v>
+      <c r="A36" s="29" t="s">
+        <v>53</v>
       </c>
       <c r="B36" s="18">
         <v>448.79</v>
@@ -1992,8 +1734,8 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="19" t="s">
-        <v>41</v>
+      <c r="A37" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="B37" s="18">
         <v>46</v>
@@ -2009,8 +1751,8 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="19" t="s">
-        <v>42</v>
+      <c r="A38" s="29" t="s">
+        <v>55</v>
       </c>
       <c r="B38" s="17"/>
       <c r="C38" s="17"/>
@@ -2024,8 +1766,8 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="14.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="19" t="s">
-        <v>43</v>
+      <c r="A39" s="29" t="s">
+        <v>56</v>
       </c>
       <c r="B39" s="10">
         <v>3000</v>
@@ -2048,7 +1790,7 @@
     </row>
     <row r="40" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B40" s="14">
         <v>3975.29</v>
@@ -2071,7 +1813,7 @@
     </row>
     <row r="41" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
@@ -2087,8 +1829,8 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="19" t="s">
-        <v>46</v>
+      <c r="A42" s="29" t="s">
+        <v>57</v>
       </c>
       <c r="B42" s="17"/>
       <c r="C42" s="17"/>
@@ -2106,8 +1848,8 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="19" t="s">
-        <v>47</v>
+      <c r="A43" s="29" t="s">
+        <v>58</v>
       </c>
       <c r="B43" s="18">
         <v>141.85</v>
@@ -2129,31 +1871,31 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="14.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="19" t="s">
-        <v>48</v>
+      <c r="A44" s="29" t="s">
+        <v>59</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
-      <c r="F44" s="21">
+      <c r="F44" s="20">
         <v>750</v>
       </c>
-      <c r="G44" s="21">
+      <c r="G44" s="20">
         <v>750</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="25">
+        <v>26</v>
+      </c>
+      <c r="B45" s="24">
         <v>141.85</v>
       </c>
-      <c r="C45" s="24">
+      <c r="C45" s="23">
         <v>181.86</v>
       </c>
-      <c r="D45" s="24">
+      <c r="D45" s="23">
         <v>629.30999999999995</v>
       </c>
       <c r="E45" s="15">
@@ -2168,7 +1910,7 @@
     </row>
     <row r="46" spans="1:7" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -2180,22 +1922,22 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="14.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B47" s="21">
+      <c r="A47" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47" s="20">
         <v>345.75</v>
       </c>
-      <c r="C47" s="21">
+      <c r="C47" s="20">
         <v>35</v>
       </c>
-      <c r="D47" s="21">
+      <c r="D47" s="20">
         <v>125</v>
       </c>
-      <c r="E47" s="21">
+      <c r="E47" s="20">
         <v>15.65</v>
       </c>
-      <c r="F47" s="21">
+      <c r="F47" s="20">
         <v>694.85</v>
       </c>
       <c r="G47" s="10">
@@ -2204,21 +1946,21 @@
     </row>
     <row r="48" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B48" s="25">
+        <v>28</v>
+      </c>
+      <c r="B48" s="24">
         <v>345.75</v>
       </c>
-      <c r="C48" s="25">
+      <c r="C48" s="24">
         <v>35</v>
       </c>
-      <c r="D48" s="25">
+      <c r="D48" s="24">
         <v>125</v>
       </c>
-      <c r="E48" s="25">
+      <c r="E48" s="24">
         <v>15.65</v>
       </c>
-      <c r="F48" s="25">
+      <c r="F48" s="24">
         <v>694.85</v>
       </c>
       <c r="G48" s="14">
@@ -2226,8 +1968,8 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
-        <v>53</v>
+      <c r="A49" s="25" t="s">
+        <v>61</v>
       </c>
       <c r="B49" s="18">
         <v>246.94</v>
@@ -2245,8 +1987,8 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="19" t="s">
-        <v>54</v>
+      <c r="A50" s="29" t="s">
+        <v>62</v>
       </c>
       <c r="B50" s="17"/>
       <c r="C50" s="18">
@@ -2260,8 +2002,8 @@
       </c>
     </row>
     <row r="51" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="19" t="s">
-        <v>55</v>
+      <c r="A51" s="29" t="s">
+        <v>63</v>
       </c>
       <c r="B51" s="17"/>
       <c r="C51" s="17"/>
@@ -2277,39 +2019,39 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="14.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="21">
+      <c r="A52" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52" s="20">
         <v>9.99</v>
       </c>
       <c r="C52" s="9"/>
-      <c r="D52" s="21">
+      <c r="D52" s="20">
         <v>28.91</v>
       </c>
       <c r="E52" s="9"/>
       <c r="F52" s="9"/>
-      <c r="G52" s="21">
+      <c r="G52" s="20">
         <v>38.9</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B53" s="25">
+        <v>29</v>
+      </c>
+      <c r="B53" s="24">
         <v>256.93</v>
       </c>
-      <c r="C53" s="25">
+      <c r="C53" s="24">
         <v>478.36</v>
       </c>
-      <c r="D53" s="25">
+      <c r="D53" s="24">
         <v>28.91</v>
       </c>
-      <c r="E53" s="25">
+      <c r="E53" s="24">
         <v>817.68</v>
       </c>
-      <c r="F53" s="25">
+      <c r="F53" s="24">
         <v>685.29</v>
       </c>
       <c r="G53" s="14">
@@ -2318,7 +2060,7 @@
     </row>
     <row r="54" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="B54" s="18">
         <v>539</v>
@@ -2341,7 +2083,7 @@
     </row>
     <row r="55" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="19" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B55" s="18">
         <v>461.35</v>
@@ -2363,8 +2105,8 @@
       </c>
     </row>
     <row r="56" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="19" t="s">
-        <v>60</v>
+      <c r="A56" s="29" t="s">
+        <v>66</v>
       </c>
       <c r="B56" s="18">
         <v>116.34</v>
@@ -2386,8 +2128,8 @@
       </c>
     </row>
     <row r="57" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="19" t="s">
-        <v>61</v>
+      <c r="A57" s="29" t="s">
+        <v>67</v>
       </c>
       <c r="B57" s="18">
         <v>727</v>
@@ -2403,37 +2145,37 @@
       </c>
     </row>
     <row r="58" spans="1:8" ht="14.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="19" t="s">
-        <v>62</v>
+      <c r="A58" s="29" t="s">
+        <v>68</v>
       </c>
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
       <c r="E58" s="9"/>
-      <c r="F58" s="21">
+      <c r="F58" s="20">
         <v>7</v>
       </c>
-      <c r="G58" s="21">
+      <c r="G58" s="20">
         <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="B59" s="11">
         <v>1843.69</v>
       </c>
-      <c r="C59" s="22">
+      <c r="C59" s="21">
         <v>808.87</v>
       </c>
-      <c r="D59" s="22">
+      <c r="D59" s="21">
         <v>765.72</v>
       </c>
-      <c r="E59" s="22">
+      <c r="E59" s="21">
         <v>756.5</v>
       </c>
-      <c r="F59" s="22">
+      <c r="F59" s="21">
         <v>697.57</v>
       </c>
       <c r="G59" s="11">
@@ -2442,7 +2184,7 @@
     </row>
     <row r="60" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="B60" s="11">
         <v>11102.54</v>
@@ -2465,7 +2207,7 @@
     </row>
     <row r="61" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="B61" s="11">
         <v>7569.97</v>
@@ -2488,7 +2230,7 @@
     </row>
     <row r="62" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="B62" s="14">
         <v>7569.97</v>
@@ -2510,16 +2252,16 @@
       </c>
     </row>
     <row r="63" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="B63" s="29"/>
-      <c r="C63" s="29"/>
-      <c r="D63" s="29"/>
-      <c r="E63" s="29"/>
-      <c r="F63" s="29"/>
-      <c r="G63" s="29"/>
-      <c r="H63" s="29"/>
+      <c r="A63" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B63" s="28"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="28"/>
+      <c r="F63" s="28"/>
+      <c r="G63" s="28"/>
+      <c r="H63" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>